<commit_message>
Data intake test 05-29_17-17
</commit_message>
<xml_diff>
--- a/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
+++ b/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
@@ -56,7 +56,7 @@
     <t xml:space="preserve">2 IST</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Conversion Test 05-29_17-14</t>
+    <t xml:space="preserve">Data Conversion Test 05-29_17-17</t>
   </si>
   <si>
     <t xml:space="preserve">U.S.</t>
@@ -137,118 +137,118 @@
     <t xml:space="preserve">33-3051</t>
   </si>
   <si>
+    <t xml:space="preserve">33-9021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private Detectives and Investigators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33-3011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bailiffs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33-1011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First-Line Supervisors of Correctional Officers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2EHFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Development and Family Studies (Associate in Science)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-1093</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social and Human Service Assistants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preschool Teachers, Except Special Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25-9045</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teaching Assistants, Except Postsecondary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2LHRAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labor and Human Resources (Associate in Science)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-1071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Resources Specialists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13-1075</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Labor Relations Specialists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43-4161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human Resources Assistants, Except Payroll and Timekeeping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 IST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Sciences and Technology (Bachelor of Science)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-3021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer and Information Systems Managers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-1254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Developers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-1243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Architects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-1242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database Administrators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network and Computer Systems Administrators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-1251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Programmers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4CRMJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criminal Justice (Bachelor of Science)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Police and Sheriff's Patrol Officers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33-9021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private Detectives and Investigators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33-3011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bailiffs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33-1011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First-Line Supervisors of Correctional Officers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2EHFS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human Development and Family Studies (Associate in Science)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-1093</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social and Human Service Assistants</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25-2011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preschool Teachers, Except Special Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25-9045</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teaching Assistants, Except Postsecondary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2LHRAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Labor and Human Resources (Associate in Science)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13-1071</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human Resources Specialists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13-1075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Labor Relations Specialists</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43-4161</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human Resources Assistants, Except Payroll and Timekeeping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 IST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information Sciences and Technology (Bachelor of Science)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11-3021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer and Information Systems Managers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15-1254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Developers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15-1243</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database Architects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15-1242</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database Administrators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network and Computer Systems Administrators</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15-1251</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer Programmers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4CRMJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Criminal Justice (Bachelor of Science)</t>
   </si>
   <si>
     <t xml:space="preserve">33-3021</t>
@@ -3122,7 +3122,7 @@
   <dimension ref="A1:J299"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="G11" activeCellId="6" sqref="D5 D8 D13 D19 D24 G3 G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3459,7 +3459,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="H11" s="7" t="n">
         <v>646310</v>
@@ -3486,10 +3486,10 @@
         <v>12</v>
       </c>
       <c r="F12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="H12" s="7" t="n">
         <v>34600</v>
@@ -3516,10 +3516,10 @@
         <v>12</v>
       </c>
       <c r="F13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="H13" s="7" t="n">
         <v>15900</v>
@@ -3546,10 +3546,10 @@
         <v>12</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="H14" s="7" t="n">
         <v>52280</v>
@@ -3563,23 +3563,23 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="G15" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="H15" s="7" t="n">
         <v>409310</v>
@@ -3593,23 +3593,23 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="H16" s="7" t="n">
         <v>430240</v>
@@ -3623,23 +3623,23 @@
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="n">
         <v>25</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="H17" s="7" t="n">
         <v>1337320</v>
@@ -3653,23 +3653,23 @@
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" s="6" t="n">
         <v>2650</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="H18" s="7" t="n">
         <v>895970</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="n">
@@ -3696,10 +3696,10 @@
         <v>12</v>
       </c>
       <c r="F19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="H19" s="7" t="n">
         <v>62800</v>
@@ -3713,23 +3713,23 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="n">
         <v>2650</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="H20" s="7" t="n">
         <v>101440</v>
@@ -3743,23 +3743,23 @@
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="n">
         <v>40</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="5" t="s">
+      <c r="G21" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H21" s="7" t="n">
         <v>592600</v>
@@ -3773,23 +3773,23 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="n">
         <v>40</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="H22" s="7" t="n">
         <v>85350</v>
@@ -3803,23 +3803,23 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="6" t="n">
         <v>40</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="H23" s="7" t="n">
         <v>59920</v>
@@ -3833,7 +3833,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="6" t="n">
@@ -3846,10 +3846,10 @@
         <v>12</v>
       </c>
       <c r="F24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="H24" s="7" t="n">
         <v>76140</v>
@@ -3863,14 +3863,14 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="6" t="n">
         <v>40</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>12</v>
@@ -3879,7 +3879,7 @@
         <v>16</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H25" s="7" t="n">
         <v>323020</v>
@@ -3893,23 +3893,23 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="6" t="n">
         <v>40</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="H26" s="7" t="n">
         <v>120370</v>
@@ -3923,14 +3923,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="6" t="n">
         <v>34</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>12</v>
@@ -3939,7 +3939,7 @@
         <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="H27" s="7" t="n">
         <v>646310</v>
@@ -3953,14 +3953,14 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="6" t="n">
         <v>34</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>12</v>
@@ -3983,23 +3983,23 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="6" t="n">
         <v>34</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="H29" s="7" t="n">
         <v>52280</v>
@@ -4380,10 +4380,10 @@
         <v>12</v>
       </c>
       <c r="F42" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="H42" s="7" t="n">
         <v>120370</v>
@@ -4950,10 +4950,10 @@
         <v>12</v>
       </c>
       <c r="F61" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H61" s="7" t="n">
         <v>592600</v>
@@ -5038,10 +5038,10 @@
         <v>12</v>
       </c>
       <c r="F64" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G64" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G64" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H64" s="7" t="n">
         <v>592600</v>
@@ -5122,10 +5122,10 @@
         <v>12</v>
       </c>
       <c r="F67" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G67" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="H67" s="7" t="n">
         <v>59920</v>
@@ -5150,10 +5150,10 @@
         <v>12</v>
       </c>
       <c r="F68" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G68" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="H68" s="7" t="n">
         <v>76140</v>
@@ -5262,10 +5262,10 @@
         <v>12</v>
       </c>
       <c r="F72" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G72" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="H72" s="7" t="n">
         <v>59920</v>
@@ -5618,10 +5618,10 @@
         <v>12</v>
       </c>
       <c r="F84" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G84" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G84" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H84" s="7" t="n">
         <v>592600</v>
@@ -5674,10 +5674,10 @@
         <v>12</v>
       </c>
       <c r="F86" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G86" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="G86" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="H86" s="7" t="n">
         <v>59920</v>
@@ -6498,10 +6498,10 @@
         <v>12</v>
       </c>
       <c r="F114" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G114" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="G114" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="H114" s="7" t="n">
         <v>59920</v>
@@ -6526,10 +6526,10 @@
         <v>12</v>
       </c>
       <c r="F115" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G115" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="G115" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="H115" s="7" t="n">
         <v>76140</v>
@@ -7156,10 +7156,10 @@
         <v>12</v>
       </c>
       <c r="F136" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G136" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="G136" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="H136" s="7" t="n">
         <v>409310</v>
@@ -7186,10 +7186,10 @@
         <v>12</v>
       </c>
       <c r="F137" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G137" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="G137" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="H137" s="7" t="n">
         <v>430240</v>
@@ -7930,10 +7930,10 @@
         <v>12</v>
       </c>
       <c r="F162" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G162" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G162" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H162" s="7" t="n">
         <v>592600</v>
@@ -8140,10 +8140,10 @@
         <v>12</v>
       </c>
       <c r="F169" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G169" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="G169" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="H169" s="7" t="n">
         <v>895970</v>
@@ -8260,10 +8260,10 @@
         <v>12</v>
       </c>
       <c r="F173" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G173" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="G173" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="H173" s="7" t="n">
         <v>62800</v>
@@ -8290,10 +8290,10 @@
         <v>12</v>
       </c>
       <c r="F174" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G174" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="G174" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="H174" s="7" t="n">
         <v>895970</v>
@@ -8410,10 +8410,10 @@
         <v>12</v>
       </c>
       <c r="F178" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G178" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="G178" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="H178" s="7" t="n">
         <v>62800</v>
@@ -11461,7 +11461,7 @@
         <v>16</v>
       </c>
       <c r="G280" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H280" s="7" t="n">
         <v>323020</v>
@@ -11668,10 +11668,10 @@
         <v>12</v>
       </c>
       <c r="F287" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G287" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G287" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H287" s="7" t="n">
         <v>592600</v>
@@ -11989,7 +11989,7 @@
   <dimension ref="A1:E539"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="7" sqref="D5 D8 D13 D19 D24 G3 G11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12321,14 +12321,14 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="22" t="n">
         <v>25</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>515</v>
@@ -12336,14 +12336,14 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="22" t="n">
         <v>25</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E23" s="21" t="s">
         <v>516</v>
@@ -12351,14 +12351,14 @@
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="22" t="n">
         <v>25</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>517</v>
@@ -12366,14 +12366,14 @@
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="22" t="n">
         <v>25</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E25" s="21" t="s">
         <v>518</v>
@@ -12381,14 +12381,14 @@
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="22" t="n">
         <v>25</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E26" s="21" t="s">
         <v>519</v>
@@ -12396,14 +12396,14 @@
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="22" t="n">
         <v>2650</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E27" s="21" t="s">
         <v>520</v>
@@ -12411,14 +12411,14 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="22" t="n">
         <v>2650</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E28" s="21" t="s">
         <v>521</v>
@@ -12426,14 +12426,14 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="22" t="n">
         <v>2650</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E29" s="21" t="s">
         <v>522</v>
@@ -12441,14 +12441,14 @@
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="22" t="n">
         <v>2650</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" s="21" t="s">
         <v>523</v>
@@ -12456,14 +12456,14 @@
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="22" t="n">
         <v>40</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" s="21" t="s">
         <v>524</v>
@@ -12471,14 +12471,14 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="22" t="n">
         <v>40</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>525</v>
@@ -12486,14 +12486,14 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="22" t="n">
         <v>40</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E33" s="21" t="s">
         <v>526</v>
@@ -12501,14 +12501,14 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="22" t="n">
         <v>40</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34" s="21" t="s">
         <v>527</v>
@@ -12516,14 +12516,14 @@
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="22" t="n">
         <v>40</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="21" t="s">
         <v>528</v>
@@ -12531,14 +12531,14 @@
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="22" t="n">
         <v>40</v>
       </c>
       <c r="D36" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E36" s="21" t="s">
         <v>529</v>
@@ -12546,14 +12546,14 @@
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="22" t="n">
         <v>34</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E37" s="21" t="s">
         <v>511</v>
@@ -12561,14 +12561,14 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="22" t="n">
         <v>34</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E38" s="21" t="s">
         <v>530</v>
@@ -12576,14 +12576,14 @@
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="22" t="n">
         <v>34</v>
       </c>
       <c r="D39" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E39" s="21" t="s">
         <v>531</v>
@@ -12591,14 +12591,14 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="22" t="n">
         <v>34</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E40" s="21" t="s">
         <v>532</v>

</xml_diff>

<commit_message>
Data intake process test, intake branch 05-29_17-32
</commit_message>
<xml_diff>
--- a/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
+++ b/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
@@ -56,7 +56,7 @@
     <t xml:space="preserve">2 IST</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Conversion Test 05-29_17-17</t>
+    <t xml:space="preserve">Data Conversion Test 05-29_17-30</t>
   </si>
   <si>
     <t xml:space="preserve">U.S.</t>
@@ -3122,7 +3122,7 @@
   <dimension ref="A1:J299"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="6" sqref="D5 D8 D13 D19 D24 G3 G11"/>
+      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11989,7 +11989,7 @@
   <dimension ref="A1:E539"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="7" sqref="D5 D8 D13 D19 D24 G3 G11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Data intake process test 05-29_18-03 intake
</commit_message>
<xml_diff>
--- a/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
+++ b/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
@@ -56,7 +56,7 @@
     <t xml:space="preserve">2 IST</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Conversion Test 05-29_17-17</t>
+    <t xml:space="preserve">Data Conversion Test 05-29_18_03</t>
   </si>
   <si>
     <t xml:space="preserve">U.S.</t>
@@ -3122,14 +3122,14 @@
   <dimension ref="A1:J299"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="6" sqref="D5 D8 D13 D19 D24 G3 G11"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="6" sqref="D5 D8 D13 D19 D24 G11 G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="59.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="59.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="41.14"/>
@@ -11989,10 +11989,10 @@
   <dimension ref="A1:E539"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="7" sqref="D5 D8 D13 D19 D24 G3 G11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="7" sqref="D5 D8 D13 D19 D24 G11 G3 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.71"/>

</xml_diff>

<commit_message>
Update BLS data (test)
</commit_message>
<xml_diff>
--- a/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
+++ b/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
@@ -2774,8 +2774,8 @@
   </sheetPr>
   <dimension ref="A1:J281"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H42" activeCellId="0" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3711,7 +3711,7 @@
         <v>84</v>
       </c>
       <c r="H31" s="4" t="n">
-        <v>666990</v>
+        <v>238497987</v>
       </c>
       <c r="I31" s="3" t="n">
         <v>0.039</v>
@@ -3981,7 +3981,7 @@
         <v>94</v>
       </c>
       <c r="H40" s="4" t="n">
-        <v>110790</v>
+        <v>234</v>
       </c>
       <c r="I40" s="3" t="n">
         <v>0.023</v>

</xml_diff>

<commit_message>
Update BLS data 2025-08-21-14-51-55 (#25)
* Update BLS data (test)

* Update BLS JSON files 2025-08-21-14-51-55

* Update BLS data (test)

* Update BLS JSON files 2025-08-21-15-03-16

* Update BLS data (test)

* Update BLS JSON files 2025-08-21-15-17-51

* Update BLS data (test)

* Update BLS JSON files 2025-08-21-15-29-04

---------

Co-authored-by: Zachary Ishler <zri5004@psu.edu>
Co-authored-by: github-actions[bot] <github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
+++ b/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
@@ -2774,8 +2774,8 @@
   </sheetPr>
   <dimension ref="A1:J281"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3291,7 +3291,7 @@
         <v>50</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>60730</v>
+        <v>234235</v>
       </c>
       <c r="I17" s="3" t="n">
         <v>0.131</v>
@@ -3351,7 +3351,7 @@
         <v>56</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>2312</v>
+        <v>3584420</v>
       </c>
       <c r="I19" s="3" t="n">
         <v>0.058</v>
@@ -3381,7 +3381,7 @@
         <v>60</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>893900</v>
+        <v>234234234</v>
       </c>
       <c r="I20" s="3" t="n">
         <v>0.106</v>
@@ -3411,7 +3411,7 @@
         <v>62</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>122</v>
+        <v>211850</v>
       </c>
       <c r="I21" s="3" t="n">
         <v>0.055</v>
@@ -3501,7 +3501,7 @@
         <v>68</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>1212</v>
+        <v>500</v>
       </c>
       <c r="I24" s="3" t="n">
         <v>0.028</v>
@@ -3591,7 +3591,7 @@
         <v>74</v>
       </c>
       <c r="H27" s="4" t="n">
-        <v>195490</v>
+        <v>3453346</v>
       </c>
       <c r="I27" s="3" t="n">
         <v>0.082</v>
@@ -3621,7 +3621,7 @@
         <v>78</v>
       </c>
       <c r="H28" s="4" t="n">
-        <v>1212</v>
+        <v>10</v>
       </c>
       <c r="I28" s="3" t="n">
         <v>0.055</v>
@@ -3681,7 +3681,7 @@
         <v>62</v>
       </c>
       <c r="H30" s="4" t="n">
-        <v>211850</v>
+        <v>12323</v>
       </c>
       <c r="I30" s="3" t="n">
         <v>0.055</v>
@@ -3711,7 +3711,7 @@
         <v>84</v>
       </c>
       <c r="H31" s="4" t="n">
-        <v>666990</v>
+        <v>342352</v>
       </c>
       <c r="I31" s="3" t="n">
         <v>0.039</v>
@@ -3741,7 +3741,7 @@
         <v>86</v>
       </c>
       <c r="H32" s="4" t="n">
-        <v>53390</v>
+        <v>17777</v>
       </c>
       <c r="I32" s="3" t="n">
         <v>-0.016</v>
@@ -3771,7 +3771,7 @@
         <v>88</v>
       </c>
       <c r="H33" s="4" t="n">
-        <v>38700</v>
+        <v>123</v>
       </c>
       <c r="I33" s="3" t="n">
         <v>0.05</v>
@@ -3801,7 +3801,7 @@
         <v>90</v>
       </c>
       <c r="H34" s="4" t="n">
-        <v>16910</v>
+        <v>346346346</v>
       </c>
       <c r="I34" s="3" t="n">
         <v>-0.014</v>
@@ -3831,7 +3831,7 @@
         <v>84</v>
       </c>
       <c r="H35" s="4" t="n">
-        <v>666990</v>
+        <v>15555</v>
       </c>
       <c r="I35" s="3" t="n">
         <v>0.039</v>
@@ -3861,7 +3861,7 @@
         <v>86</v>
       </c>
       <c r="H36" s="4" t="n">
-        <v>53390</v>
+        <v>123123123</v>
       </c>
       <c r="I36" s="3" t="n">
         <v>-0.016</v>
@@ -3891,7 +3891,7 @@
         <v>94</v>
       </c>
       <c r="H37" s="4" t="n">
-        <v>110790</v>
+        <v>234234</v>
       </c>
       <c r="I37" s="3" t="n">
         <v>0.023</v>
@@ -3921,7 +3921,7 @@
         <v>98</v>
       </c>
       <c r="H38" s="4" t="n">
-        <v>12570</v>
+        <v>666</v>
       </c>
       <c r="I38" s="3" t="n">
         <v>0.04</v>
@@ -3951,7 +3951,7 @@
         <v>100</v>
       </c>
       <c r="H39" s="4" t="n">
-        <v>86820</v>
+        <v>34</v>
       </c>
       <c r="I39" s="3" t="n">
         <v>0.036</v>
@@ -3981,7 +3981,7 @@
         <v>94</v>
       </c>
       <c r="H40" s="4" t="n">
-        <v>110790</v>
+        <v>234</v>
       </c>
       <c r="I40" s="3" t="n">
         <v>0.023</v>
@@ -4011,7 +4011,7 @@
         <v>104</v>
       </c>
       <c r="H41" s="4" t="n">
-        <v>1393310</v>
+        <v>23423423423</v>
       </c>
       <c r="I41" s="3" t="n">
         <v>-0.007</v>
@@ -4131,7 +4131,7 @@
         <v>114</v>
       </c>
       <c r="H45" s="4" t="n">
-        <v>439380</v>
+        <v>2333</v>
       </c>
       <c r="I45" s="3" t="n">
         <v>0.108</v>
@@ -4161,7 +4161,7 @@
         <v>116</v>
       </c>
       <c r="H46" s="4" t="n">
-        <v>179430</v>
+        <v>333</v>
       </c>
       <c r="I46" s="3" t="n">
         <v>0.327</v>
@@ -4191,7 +4191,7 @@
         <v>116</v>
       </c>
       <c r="H47" s="4" t="n">
-        <v>179430</v>
+        <v>333</v>
       </c>
       <c r="I47" s="3" t="n">
         <v>0.327</v>
@@ -11198,7 +11198,7 @@
   </sheetPr>
   <dimension ref="A1:E505"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A286" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E305" activeCellId="0" sqref="E305"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update BLS data (test, again)
</commit_message>
<xml_diff>
--- a/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
+++ b/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
@@ -2774,8 +2774,8 @@
   </sheetPr>
   <dimension ref="A1:J281"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H33" activeCellId="0" sqref="H33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3381,7 +3381,7 @@
         <v>60</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>893900</v>
+        <v>3423</v>
       </c>
       <c r="I20" s="3" t="n">
         <v>0.106</v>
@@ -3501,7 +3501,7 @@
         <v>68</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>1212</v>
+        <v>2323</v>
       </c>
       <c r="I24" s="3" t="n">
         <v>0.028</v>
@@ -3651,7 +3651,7 @@
         <v>80</v>
       </c>
       <c r="H29" s="4" t="n">
-        <v>100870</v>
+        <v>2323</v>
       </c>
       <c r="I29" s="3" t="n">
         <v>0.075</v>

</xml_diff>

<commit_message>
Update BLS data  (#30)
* Update BLS data (test)

* Update BLS JSON files

---------

Co-authored-by: Zachary Ishler <zri5004@psu.edu>
Co-authored-by: github-actions[bot] <github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
+++ b/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
@@ -2775,7 +2775,7 @@
   <dimension ref="A1:J281"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
+      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3771,7 +3771,7 @@
         <v>88</v>
       </c>
       <c r="H33" s="4" t="n">
-        <v>123</v>
+        <v>4234334</v>
       </c>
       <c r="I33" s="3" t="n">
         <v>0.05</v>
@@ -3921,7 +3921,7 @@
         <v>98</v>
       </c>
       <c r="H38" s="4" t="n">
-        <v>245565467567</v>
+        <v>1233</v>
       </c>
       <c r="I38" s="3" t="n">
         <v>0.04</v>

</xml_diff>

<commit_message>
Update BLS data  (#39)
</commit_message>
<xml_diff>
--- a/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
+++ b/docs/bls-data/World-Campus-BLS-Data-Latest.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2932" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2932" uniqueCount="856">
   <si>
     <t xml:space="preserve">prospect_code</t>
   </si>
@@ -2133,6 +2133,9 @@
   </si>
   <si>
     <t xml:space="preserve">Instructional Systems Specialist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning Development Specialist (Ooo! Fancy!!!!!)</t>
   </si>
   <si>
     <t xml:space="preserve">Adult Basic Education Instructor (ABE Instructor)</t>
@@ -11374,8 +11377,8 @@
   </sheetPr>
   <dimension ref="A1:E505"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A280" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E288" activeCellId="0" sqref="E288"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A286" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E286" activeCellId="0" sqref="E286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15645,7 +15648,7 @@
         <v>312</v>
       </c>
       <c r="E286" s="8" t="s">
-        <v>582</v>
+        <v>704</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15660,7 +15663,7 @@
         <v>318</v>
       </c>
       <c r="E287" s="8" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15675,7 +15678,7 @@
         <v>318</v>
       </c>
       <c r="E288" s="8" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15690,7 +15693,7 @@
         <v>318</v>
       </c>
       <c r="E289" s="8" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15705,7 +15708,7 @@
         <v>318</v>
       </c>
       <c r="E290" s="8" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15735,7 +15738,7 @@
         <v>322</v>
       </c>
       <c r="E292" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15765,7 +15768,7 @@
         <v>322</v>
       </c>
       <c r="E294" s="8" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15780,7 +15783,7 @@
         <v>322</v>
       </c>
       <c r="E295" s="8" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15795,7 +15798,7 @@
         <v>322</v>
       </c>
       <c r="E296" s="8" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15810,7 +15813,7 @@
         <v>328</v>
       </c>
       <c r="E297" s="8" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15825,7 +15828,7 @@
         <v>328</v>
       </c>
       <c r="E298" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15840,7 +15843,7 @@
         <v>328</v>
       </c>
       <c r="E299" s="8" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15855,7 +15858,7 @@
         <v>328</v>
       </c>
       <c r="E300" s="8" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15870,7 +15873,7 @@
         <v>328</v>
       </c>
       <c r="E301" s="8" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15885,7 +15888,7 @@
         <v>328</v>
       </c>
       <c r="E302" s="8" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15898,7 +15901,7 @@
         <v>330</v>
       </c>
       <c r="E303" s="8" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15911,7 +15914,7 @@
         <v>330</v>
       </c>
       <c r="E304" s="8" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15937,7 +15940,7 @@
         <v>330</v>
       </c>
       <c r="E306" s="8" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15950,7 +15953,7 @@
         <v>330</v>
       </c>
       <c r="E307" s="8" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15976,7 +15979,7 @@
         <v>330</v>
       </c>
       <c r="E309" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16002,7 +16005,7 @@
         <v>335</v>
       </c>
       <c r="E311" s="8" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16028,7 +16031,7 @@
         <v>335</v>
       </c>
       <c r="E313" s="8" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16041,7 +16044,7 @@
         <v>335</v>
       </c>
       <c r="E314" s="8" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16054,7 +16057,7 @@
         <v>335</v>
       </c>
       <c r="E315" s="8" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16067,7 +16070,7 @@
         <v>335</v>
       </c>
       <c r="E316" s="8" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16095,7 +16098,7 @@
         <v>337</v>
       </c>
       <c r="E318" s="8" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16110,7 +16113,7 @@
         <v>337</v>
       </c>
       <c r="E319" s="8" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16125,7 +16128,7 @@
         <v>337</v>
       </c>
       <c r="E320" s="8" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16155,7 +16158,7 @@
         <v>337</v>
       </c>
       <c r="E322" s="8" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16170,7 +16173,7 @@
         <v>341</v>
       </c>
       <c r="E323" s="8" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16185,7 +16188,7 @@
         <v>341</v>
       </c>
       <c r="E324" s="8" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16200,7 +16203,7 @@
         <v>341</v>
       </c>
       <c r="E325" s="8" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16215,7 +16218,7 @@
         <v>341</v>
       </c>
       <c r="E326" s="8" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="327" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16245,7 +16248,7 @@
         <v>345</v>
       </c>
       <c r="E328" s="8" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16260,7 +16263,7 @@
         <v>345</v>
       </c>
       <c r="E329" s="8" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16275,7 +16278,7 @@
         <v>345</v>
       </c>
       <c r="E330" s="8" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16290,7 +16293,7 @@
         <v>345</v>
       </c>
       <c r="E331" s="8" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16305,7 +16308,7 @@
         <v>345</v>
       </c>
       <c r="E332" s="8" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16320,7 +16323,7 @@
         <v>351</v>
       </c>
       <c r="E333" s="8" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16335,7 +16338,7 @@
         <v>351</v>
       </c>
       <c r="E334" s="8" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16350,7 +16353,7 @@
         <v>351</v>
       </c>
       <c r="E335" s="8" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16365,7 +16368,7 @@
         <v>351</v>
       </c>
       <c r="E336" s="8" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16380,7 +16383,7 @@
         <v>353</v>
       </c>
       <c r="E337" s="8" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16395,7 +16398,7 @@
         <v>353</v>
       </c>
       <c r="E338" s="8" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16410,7 +16413,7 @@
         <v>353</v>
       </c>
       <c r="E339" s="8" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16425,7 +16428,7 @@
         <v>357</v>
       </c>
       <c r="E340" s="8" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16440,7 +16443,7 @@
         <v>357</v>
       </c>
       <c r="E341" s="8" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16455,7 +16458,7 @@
         <v>357</v>
       </c>
       <c r="E342" s="8" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16470,7 +16473,7 @@
         <v>357</v>
       </c>
       <c r="E343" s="8" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16485,7 +16488,7 @@
         <v>357</v>
       </c>
       <c r="E344" s="8" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16500,7 +16503,7 @@
         <v>357</v>
       </c>
       <c r="E345" s="8" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16515,7 +16518,7 @@
         <v>359</v>
       </c>
       <c r="E346" s="8" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16530,7 +16533,7 @@
         <v>359</v>
       </c>
       <c r="E347" s="8" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16545,7 +16548,7 @@
         <v>359</v>
       </c>
       <c r="E348" s="8" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16560,7 +16563,7 @@
         <v>359</v>
       </c>
       <c r="E349" s="8" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16575,7 +16578,7 @@
         <v>359</v>
       </c>
       <c r="E350" s="8" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16590,7 +16593,7 @@
         <v>363</v>
       </c>
       <c r="E351" s="8" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16605,7 +16608,7 @@
         <v>363</v>
       </c>
       <c r="E352" s="8" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16620,7 +16623,7 @@
         <v>363</v>
       </c>
       <c r="E353" s="8" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16635,7 +16638,7 @@
         <v>363</v>
       </c>
       <c r="E354" s="8" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16650,7 +16653,7 @@
         <v>363</v>
       </c>
       <c r="E355" s="8" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16665,7 +16668,7 @@
         <v>367</v>
       </c>
       <c r="E356" s="8" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16680,7 +16683,7 @@
         <v>367</v>
       </c>
       <c r="E357" s="8" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16695,7 +16698,7 @@
         <v>367</v>
       </c>
       <c r="E358" s="8" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16710,7 +16713,7 @@
         <v>367</v>
       </c>
       <c r="E359" s="8" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16725,7 +16728,7 @@
         <v>367</v>
       </c>
       <c r="E360" s="8" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16740,7 +16743,7 @@
         <v>367</v>
       </c>
       <c r="E361" s="8" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16755,7 +16758,7 @@
         <v>367</v>
       </c>
       <c r="E362" s="8" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16770,7 +16773,7 @@
         <v>367</v>
       </c>
       <c r="E363" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16785,7 +16788,7 @@
         <v>377</v>
       </c>
       <c r="E364" s="8" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16800,7 +16803,7 @@
         <v>377</v>
       </c>
       <c r="E365" s="8" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16815,7 +16818,7 @@
         <v>377</v>
       </c>
       <c r="E366" s="8" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16830,7 +16833,7 @@
         <v>377</v>
       </c>
       <c r="E367" s="8" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16845,7 +16848,7 @@
         <v>377</v>
       </c>
       <c r="E368" s="8" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16860,7 +16863,7 @@
         <v>377</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16875,7 +16878,7 @@
         <v>377</v>
       </c>
       <c r="E370" s="8" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16890,7 +16893,7 @@
         <v>377</v>
       </c>
       <c r="E371" s="8" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16905,7 +16908,7 @@
         <v>379</v>
       </c>
       <c r="E372" s="8" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16935,7 +16938,7 @@
         <v>379</v>
       </c>
       <c r="E374" s="8" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16950,7 +16953,7 @@
         <v>379</v>
       </c>
       <c r="E375" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16965,7 +16968,7 @@
         <v>379</v>
       </c>
       <c r="E376" s="8" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16980,7 +16983,7 @@
         <v>383</v>
       </c>
       <c r="E377" s="8" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17010,7 +17013,7 @@
         <v>383</v>
       </c>
       <c r="E379" s="8" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17025,7 +17028,7 @@
         <v>383</v>
       </c>
       <c r="E380" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17040,7 +17043,7 @@
         <v>383</v>
       </c>
       <c r="E381" s="8" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17055,7 +17058,7 @@
         <v>385</v>
       </c>
       <c r="E382" s="8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17070,7 +17073,7 @@
         <v>385</v>
       </c>
       <c r="E383" s="8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17085,7 +17088,7 @@
         <v>385</v>
       </c>
       <c r="E384" s="8" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17100,7 +17103,7 @@
         <v>385</v>
       </c>
       <c r="E385" s="8" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17115,7 +17118,7 @@
         <v>385</v>
       </c>
       <c r="E386" s="8" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17130,7 +17133,7 @@
         <v>391</v>
       </c>
       <c r="E387" s="8" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17145,7 +17148,7 @@
         <v>391</v>
       </c>
       <c r="E388" s="8" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17160,7 +17163,7 @@
         <v>391</v>
       </c>
       <c r="E389" s="8" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17175,7 +17178,7 @@
         <v>391</v>
       </c>
       <c r="E390" s="8" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17190,7 +17193,7 @@
         <v>391</v>
       </c>
       <c r="E391" s="8" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17205,7 +17208,7 @@
         <v>393</v>
       </c>
       <c r="E392" s="8" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17220,7 +17223,7 @@
         <v>393</v>
       </c>
       <c r="E393" s="8" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17235,7 +17238,7 @@
         <v>393</v>
       </c>
       <c r="E394" s="8" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17265,7 +17268,7 @@
         <v>393</v>
       </c>
       <c r="E396" s="8" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17280,7 +17283,7 @@
         <v>393</v>
       </c>
       <c r="E397" s="8" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17295,7 +17298,7 @@
         <v>399</v>
       </c>
       <c r="E398" s="8" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17310,7 +17313,7 @@
         <v>399</v>
       </c>
       <c r="E399" s="8" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17325,7 +17328,7 @@
         <v>399</v>
       </c>
       <c r="E400" s="8" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17340,7 +17343,7 @@
         <v>399</v>
       </c>
       <c r="E401" s="8" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17370,7 +17373,7 @@
         <v>401</v>
       </c>
       <c r="E403" s="8" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="404" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17385,7 +17388,7 @@
         <v>401</v>
       </c>
       <c r="E404" s="8" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17400,7 +17403,7 @@
         <v>401</v>
       </c>
       <c r="E405" s="8" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17415,7 +17418,7 @@
         <v>401</v>
       </c>
       <c r="E406" s="8" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17445,7 +17448,7 @@
         <v>405</v>
       </c>
       <c r="E408" s="8" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17460,7 +17463,7 @@
         <v>405</v>
       </c>
       <c r="E409" s="8" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17475,7 +17478,7 @@
         <v>405</v>
       </c>
       <c r="E410" s="8" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17490,7 +17493,7 @@
         <v>405</v>
       </c>
       <c r="E411" s="8" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17520,7 +17523,7 @@
         <v>407</v>
       </c>
       <c r="E413" s="8" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17550,7 +17553,7 @@
         <v>407</v>
       </c>
       <c r="E415" s="8" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17565,7 +17568,7 @@
         <v>407</v>
       </c>
       <c r="E416" s="8" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17610,7 +17613,7 @@
         <v>411</v>
       </c>
       <c r="E419" s="8" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17625,7 +17628,7 @@
         <v>411</v>
       </c>
       <c r="E420" s="8" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17640,7 +17643,7 @@
         <v>411</v>
       </c>
       <c r="E421" s="8" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17655,7 +17658,7 @@
         <v>411</v>
       </c>
       <c r="E422" s="8" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17667,10 +17670,10 @@
         <v>2542</v>
       </c>
       <c r="D423" s="8" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E423" s="8" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17682,10 +17685,10 @@
         <v>2542</v>
       </c>
       <c r="D424" s="8" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E424" s="8" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17697,10 +17700,10 @@
         <v>2542</v>
       </c>
       <c r="D425" s="8" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E425" s="8" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17712,10 +17715,10 @@
         <v>2542</v>
       </c>
       <c r="D426" s="8" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E426" s="8" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17727,10 +17730,10 @@
         <v>2542</v>
       </c>
       <c r="D427" s="8" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E427" s="8" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17745,7 +17748,7 @@
         <v>418</v>
       </c>
       <c r="E428" s="8" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17790,7 +17793,7 @@
         <v>418</v>
       </c>
       <c r="E431" s="8" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17805,7 +17808,7 @@
         <v>418</v>
       </c>
       <c r="E432" s="8" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17820,7 +17823,7 @@
         <v>418</v>
       </c>
       <c r="E433" s="8" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17835,7 +17838,7 @@
         <v>420</v>
       </c>
       <c r="E434" s="8" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17865,7 +17868,7 @@
         <v>420</v>
       </c>
       <c r="E436" s="8" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17910,7 +17913,7 @@
         <v>422</v>
       </c>
       <c r="E439" s="8" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17925,7 +17928,7 @@
         <v>422</v>
       </c>
       <c r="E440" s="8" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17940,7 +17943,7 @@
         <v>422</v>
       </c>
       <c r="E441" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17955,7 +17958,7 @@
         <v>422</v>
       </c>
       <c r="E442" s="8" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17970,7 +17973,7 @@
         <v>422</v>
       </c>
       <c r="E443" s="8" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17985,7 +17988,7 @@
         <v>426</v>
       </c>
       <c r="E444" s="8" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18000,7 +18003,7 @@
         <v>426</v>
       </c>
       <c r="E445" s="8" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18015,7 +18018,7 @@
         <v>426</v>
       </c>
       <c r="E446" s="8" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18030,7 +18033,7 @@
         <v>426</v>
       </c>
       <c r="E447" s="8" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18060,7 +18063,7 @@
         <v>428</v>
       </c>
       <c r="E449" s="8" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18090,7 +18093,7 @@
         <v>428</v>
       </c>
       <c r="E451" s="8" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18105,7 +18108,7 @@
         <v>428</v>
       </c>
       <c r="E452" s="8" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18120,7 +18123,7 @@
         <v>428</v>
       </c>
       <c r="E453" s="8" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18135,7 +18138,7 @@
         <v>430</v>
       </c>
       <c r="E454" s="8" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18150,7 +18153,7 @@
         <v>430</v>
       </c>
       <c r="E455" s="8" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18165,7 +18168,7 @@
         <v>430</v>
       </c>
       <c r="E456" s="8" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18180,7 +18183,7 @@
         <v>430</v>
       </c>
       <c r="E457" s="8" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18195,7 +18198,7 @@
         <v>430</v>
       </c>
       <c r="E458" s="8" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18210,7 +18213,7 @@
         <v>440</v>
       </c>
       <c r="E459" s="8" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18225,7 +18228,7 @@
         <v>440</v>
       </c>
       <c r="E460" s="8" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18240,7 +18243,7 @@
         <v>440</v>
       </c>
       <c r="E461" s="8" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18255,7 +18258,7 @@
         <v>440</v>
       </c>
       <c r="E462" s="8" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18270,7 +18273,7 @@
         <v>440</v>
       </c>
       <c r="E463" s="8" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18285,7 +18288,7 @@
         <v>440</v>
       </c>
       <c r="E464" s="8" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18300,7 +18303,7 @@
         <v>442</v>
       </c>
       <c r="E465" s="8" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18315,7 +18318,7 @@
         <v>442</v>
       </c>
       <c r="E466" s="8" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18330,7 +18333,7 @@
         <v>442</v>
       </c>
       <c r="E467" s="8" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18345,7 +18348,7 @@
         <v>442</v>
       </c>
       <c r="E468" s="8" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18360,7 +18363,7 @@
         <v>442</v>
       </c>
       <c r="E469" s="8" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18420,7 +18423,7 @@
         <v>444</v>
       </c>
       <c r="E473" s="8" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18435,7 +18438,7 @@
         <v>444</v>
       </c>
       <c r="E474" s="8" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18450,7 +18453,7 @@
         <v>446</v>
       </c>
       <c r="E475" s="8" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18465,7 +18468,7 @@
         <v>446</v>
       </c>
       <c r="E476" s="8" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18480,7 +18483,7 @@
         <v>446</v>
       </c>
       <c r="E477" s="8" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="478" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18495,7 +18498,7 @@
         <v>446</v>
       </c>
       <c r="E478" s="8" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18510,7 +18513,7 @@
         <v>446</v>
       </c>
       <c r="E479" s="8" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18555,7 +18558,7 @@
         <v>448</v>
       </c>
       <c r="E482" s="8" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18570,7 +18573,7 @@
         <v>448</v>
       </c>
       <c r="E483" s="8" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18585,7 +18588,7 @@
         <v>448</v>
       </c>
       <c r="E484" s="8" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18615,7 +18618,7 @@
         <v>448</v>
       </c>
       <c r="E486" s="8" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18630,7 +18633,7 @@
         <v>448</v>
       </c>
       <c r="E487" s="8" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18645,7 +18648,7 @@
         <v>448</v>
       </c>
       <c r="E488" s="8" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18660,7 +18663,7 @@
         <v>448</v>
       </c>
       <c r="E489" s="8" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18675,7 +18678,7 @@
         <v>454</v>
       </c>
       <c r="E490" s="8" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18690,7 +18693,7 @@
         <v>454</v>
       </c>
       <c r="E491" s="8" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18705,7 +18708,7 @@
         <v>454</v>
       </c>
       <c r="E492" s="8" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18720,7 +18723,7 @@
         <v>454</v>
       </c>
       <c r="E493" s="8" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18735,7 +18738,7 @@
         <v>454</v>
       </c>
       <c r="E494" s="8" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18750,7 +18753,7 @@
         <v>462</v>
       </c>
       <c r="E495" s="8" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18765,7 +18768,7 @@
         <v>462</v>
       </c>
       <c r="E496" s="8" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18780,7 +18783,7 @@
         <v>462</v>
       </c>
       <c r="E497" s="8" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18795,7 +18798,7 @@
         <v>462</v>
       </c>
       <c r="E498" s="8" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
     </row>
     <row r="499" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18810,7 +18813,7 @@
         <v>462</v>
       </c>
       <c r="E499" s="8" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18825,7 +18828,7 @@
         <v>466</v>
       </c>
       <c r="E500" s="8" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18840,7 +18843,7 @@
         <v>466</v>
       </c>
       <c r="E501" s="8" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18855,7 +18858,7 @@
         <v>466</v>
       </c>
       <c r="E502" s="8" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18870,7 +18873,7 @@
         <v>466</v>
       </c>
       <c r="E503" s="8" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18885,7 +18888,7 @@
         <v>466</v>
       </c>
       <c r="E504" s="8" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18900,7 +18903,7 @@
         <v>466</v>
       </c>
       <c r="E505" s="8" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>